<commit_message>
Add DateTime and error columns to Excel test file
</commit_message>
<xml_diff>
--- a/test/TestData.xlsx
+++ b/test/TestData.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Some Float64s</t>
   </si>
@@ -75,12 +78,27 @@
   </si>
   <si>
     <t>III</t>
+  </si>
+  <si>
+    <t>Some dates</t>
+  </si>
+  <si>
+    <t>Some errors</t>
+  </si>
+  <si>
+    <t>Dates with NA</t>
+  </si>
+  <si>
+    <t>Errors with NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,8 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -127,6 +149,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="nonexistingsheet"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -392,15 +427,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J7"/>
+  <dimension ref="C3:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G7"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.58203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -425,8 +472,20 @@
       <c r="J3" t="s">
         <v>6</v>
       </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C4">
         <v>1</v>
       </c>
@@ -448,8 +507,22 @@
       <c r="I4" t="s">
         <v>13</v>
       </c>
+      <c r="K4" s="1">
+        <v>42066</v>
+      </c>
+      <c r="L4" s="1">
+        <v>23835</v>
+      </c>
+      <c r="M4" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N4" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C5">
         <v>1.5</v>
       </c>
@@ -468,8 +541,22 @@
       <c r="J5" t="b">
         <v>1</v>
       </c>
+      <c r="K5" s="2">
+        <v>42039.426388888889</v>
+      </c>
+      <c r="L5" s="2">
+        <v>18484.777777777777</v>
+      </c>
+      <c r="M5" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N5" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C6">
         <v>2</v>
       </c>
@@ -488,8 +575,22 @@
       <c r="I6" t="s">
         <v>14</v>
       </c>
+      <c r="K6" s="2">
+        <v>32242</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="M6" t="e">
+        <f>[1]nonexistingsheet!A1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N6" t="e">
+        <f>a0</f>
+        <v>#NAME?</v>
+      </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C7">
         <v>2.5</v>
       </c>
@@ -513,6 +614,13 @@
       </c>
       <c r="J7" t="b">
         <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.62638888888888888</v>
+      </c>
+      <c r="M7" t="e">
+        <f>a0</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more test data to TestData.xlsx
</commit_message>
<xml_diff>
--- a/test/TestData.xlsx
+++ b/test/TestData.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23938" windowHeight="9210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23938" windowHeight="9210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Second Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Some Float64s</t>
   </si>
@@ -429,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,4 +627,111 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D8:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>9</v>
+      </c>
+      <c r="I9" s="1">
+        <v>42066</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>1.5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2">
+        <v>42039.426388888889</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>32242</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <v>2.5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.62638888888888888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add empty sheet to TestData.xlsx
</commit_message>
<xml_diff>
--- a/test/TestData.xlsx
+++ b/test/TestData.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23938" windowHeight="9210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23938" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Second Sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Empty Sheet" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
@@ -430,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K4" sqref="K4:K7"/>
     </sheetView>
   </sheetViews>
@@ -633,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D8:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -734,4 +735,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add another column to TestData.xlsx
</commit_message>
<xml_diff>
--- a/test/TestData.xlsx
+++ b/test/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Some Float64s</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>Errors with NA</t>
+  </si>
+  <si>
+    <t>Column with NULL and then mixed</t>
+  </si>
+  <si>
+    <t>HKEJW</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:N7"/>
+  <dimension ref="C3:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K7"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,9 +453,10 @@
     <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="13.25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -486,8 +493,11 @@
       <c r="N3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C4">
         <v>1</v>
       </c>
@@ -524,7 +534,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C5">
         <v>1.5</v>
       </c>
@@ -557,8 +567,11 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="O5">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C6">
         <v>2</v>
       </c>
@@ -591,8 +604,11 @@
         <f>a0</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="O6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C7">
         <v>2.5</v>
       </c>

</xml_diff>

<commit_message>
Add more test data to the Excel file
</commit_message>
<xml_diff>
--- a/test/TestData.xlsx
+++ b/test/TestData.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\.julia\v0.3\ExcelReaders\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anthoff\.julia\v0.4\ExcelReaders\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23938" windowHeight="9210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23940" windowHeight="9210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Second Sheet" sheetId="2" r:id="rId2"/>
-    <sheet name="Empty Sheet" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Empty Sheet" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Some Float64s</t>
   </si>
@@ -98,12 +99,18 @@
   </si>
   <si>
     <t>HKEJW</t>
+  </si>
+  <si>
+    <t>Col1</t>
+  </si>
+  <si>
+    <t>Col3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -437,26 +444,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.58203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.58203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -497,7 +504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
@@ -534,7 +541,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1.5</v>
       </c>
@@ -571,7 +578,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>2</v>
       </c>
@@ -608,7 +615,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>2.5</v>
       </c>
@@ -654,16 +661,16 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>0</v>
       </c>
@@ -680,7 +687,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>1</v>
       </c>
@@ -697,7 +704,7 @@
         <v>42066</v>
       </c>
     </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>1.5</v>
       </c>
@@ -714,10 +721,10 @@
         <v>42039.426388888889</v>
       </c>
     </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>2</v>
       </c>
@@ -731,7 +738,7 @@
         <v>32242</v>
       </c>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>2.5</v>
       </c>
@@ -755,11 +762,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>35</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>